<commit_message>
add badge frontend to the the github remie
</commit_message>
<xml_diff>
--- a/sample files/movies.xlsx
+++ b/sample files/movies.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25023"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C74C421D-9ECA-4268-98B5-C24D8A3BA90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a896199\Documents\Dev\github test app\angular-excel-csv\sample files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDC27D0-3CCE-48E5-8F7F-BFE10840534A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Movie</t>
   </si>
@@ -104,13 +109,55 @@
   </si>
   <si>
     <t>Peter Weir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2500000100048004NON10O003400000NN0O 01320000000020200100                        1333100          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2500000200048004NON10O003400000NN0O 01320002000020200100                        1333100          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2500000300048004NON10O003400000NN0O 01320002222220200100                        1333100          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2500000400048004NON10O003400000NN0O 01320002222220200100                        1333100          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2500000500048004NON10O003400000NN0O 01320002202220000100                        1333100          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2500000600048004NON10O003400000NN0O 01320002202220000100                        1333100          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2500000700048004NON10O003400000NN0O 01320002222222200100                        1333100          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2500000800048004NON10O003400000NN0O 01320002202220000100                        1333100          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2500000900048004NON10O003400000NN0O 01320002202220000100                        1333100          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2500001000048004NON10O003400000NN0O 01320002202220000100                        1333100          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2500002000048004NON10O003400000NN0O 01320002202222200100                        1333100          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2500004000048004NON10O003400000NN0O 01320002202220000100                        1333100          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2500004100048004NON10O003400000NN0O 01320002202220000100                        1333100          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2500000100049125NON10O003400000NN0O 01320002202220000100                        1333100          </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,7 +206,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -455,21 +502,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="84.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,7 +530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -497,7 +544,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -511,7 +558,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -525,7 +572,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -539,7 +586,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -553,7 +600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -567,7 +614,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -581,7 +628,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -595,7 +642,78 @@
         <v>7.3</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>